<commit_message>
feat: Add core application modules, tests, structured reporting, and documentation, while removing temporary files.
</commit_message>
<xml_diff>
--- a/data/parameters_config/project_parameters.xlsx
+++ b/data/parameters_config/project_parameters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="99">
   <si>
     <t>Category</t>
   </si>
@@ -55,6 +55,9 @@
     <t>Transport Settings</t>
   </si>
   <si>
+    <t>General Settings</t>
+  </si>
+  <si>
     <t>DECIMALS</t>
   </si>
   <si>
@@ -217,6 +220,9 @@
     <t>TRUCK_CAPACITY_T</t>
   </si>
   <si>
+    <t>Default IGU Service Lifetime (years)</t>
+  </si>
+  <si>
     <t>igu-reuse-tool/0.1 (CHANGE_THIS_TO_YOUR_EMAIL@DOMAIN)</t>
   </si>
   <si>
@@ -302,6 +308,9 @@
   </si>
   <si>
     <t>Truck emission factor (kgCO2e/tkm)</t>
+  </si>
+  <si>
+    <t>Default age assumption for IGUs at end-of-life</t>
   </si>
 </sst>
 </file>
@@ -659,7 +668,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -684,13 +693,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -698,13 +707,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>2500</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -712,13 +721,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -726,13 +735,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -740,13 +749,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -754,13 +763,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>1400</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -768,13 +777,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>0.05</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -782,13 +791,13 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>0.77</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -796,13 +805,13 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>1.29</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -810,13 +819,13 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11">
         <v>4.683</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -824,13 +833,13 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -838,13 +847,13 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13">
         <v>0.57</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -852,13 +861,13 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14">
         <v>0.17</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -866,13 +875,13 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15">
         <v>0.14</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -880,13 +889,13 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16">
         <v>0.27</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -894,13 +903,13 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <v>0.3</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -908,13 +917,13 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>0.39</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -922,13 +931,13 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19">
         <v>24000</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -936,13 +945,13 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>0.05</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -950,13 +959,13 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -964,13 +973,13 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C22">
         <v>0.15</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -978,13 +987,13 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C23">
         <v>0.15</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -992,13 +1001,13 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1006,13 +1015,13 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C25">
         <v>1.5</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1020,13 +1029,13 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1034,13 +1043,13 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1048,13 +1057,13 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1062,13 +1071,13 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1076,13 +1085,13 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1090,13 +1099,13 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C31">
         <v>0.01</v>
       </c>
       <c r="D31" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1104,13 +1113,13 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C32">
         <v>0.02</v>
       </c>
       <c r="D32" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1118,13 +1127,13 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C33">
         <v>0.95</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1132,13 +1141,13 @@
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C34">
         <v>0.9</v>
       </c>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1146,13 +1155,13 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C35">
         <v>0.1</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1160,13 +1169,13 @@
         <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C36">
         <v>0.2</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1174,13 +1183,13 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C37">
         <v>0.2</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1188,13 +1197,13 @@
         <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C38">
         <v>0.8</v>
       </c>
       <c r="D38" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1202,13 +1211,13 @@
         <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C39">
         <v>0.1</v>
       </c>
       <c r="D39" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1216,13 +1225,13 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C40">
         <v>0.1</v>
       </c>
       <c r="D40" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1230,13 +1239,13 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C41">
         <v>30</v>
       </c>
       <c r="D41" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1244,13 +1253,13 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1258,13 +1267,13 @@
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C43">
         <v>100</v>
       </c>
       <c r="D43" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1272,13 +1281,13 @@
         <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C44">
         <v>150</v>
       </c>
       <c r="D44" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1286,13 +1295,13 @@
         <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C45">
         <v>80</v>
       </c>
       <c r="D45" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1300,13 +1309,13 @@
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C46" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D46" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1314,13 +1323,13 @@
         <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C47">
         <v>1.6</v>
       </c>
       <c r="D47" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1328,13 +1337,13 @@
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C48">
         <v>50</v>
       </c>
       <c r="D48" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1342,13 +1351,13 @@
         <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C49">
         <v>100</v>
       </c>
       <c r="D49" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1356,13 +1365,13 @@
         <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C50">
         <v>0.015</v>
       </c>
       <c r="D50" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1370,13 +1379,13 @@
         <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C51">
         <v>0.062</v>
       </c>
       <c r="D51" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1384,13 +1393,13 @@
         <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C52">
         <v>500</v>
       </c>
       <c r="D52" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1398,13 +1407,13 @@
         <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C53" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D53" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1412,13 +1421,13 @@
         <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C54" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D54" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1426,13 +1435,27 @@
         <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C55">
         <v>24</v>
       </c>
       <c r="D55" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56">
+        <v>25</v>
+      </c>
+      <c r="D56" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to closed-loop recycling processes and excluding landfill and open-loop recycling from analysis
</commit_message>
<xml_diff>
--- a/data/parameters_config/project_parameters.xlsx
+++ b/data/parameters_config/project_parameters.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhartwell/PycharmProjects/VITRIFY/data/parameters_config/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A099CE67-489A-4C4D-B5F2-B67F4C7D7B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="101">
   <si>
     <t>Category</t>
   </si>
@@ -311,13 +330,19 @@
   </si>
   <si>
     <t>Default age assumption for IGUs at end-of-life</t>
+  </si>
+  <si>
+    <t>FLOAT_GLASS_REPROCESSING</t>
+  </si>
+  <si>
+    <t>Embodied Carbon: Reprocessing Flat Glass (kgCO2e/kg)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,13 +405,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -424,7 +457,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -458,6 +491,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -492,9 +526,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -667,14 +702,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,7 +728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -702,7 +742,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -716,7 +756,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -730,7 +770,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -744,7 +784,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -758,7 +798,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -772,7 +812,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -786,7 +826,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -800,7 +840,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -814,7 +854,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -822,13 +862,13 @@
         <v>23</v>
       </c>
       <c r="C11">
-        <v>4.683</v>
+        <v>4.6829999999999998</v>
       </c>
       <c r="D11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -842,7 +882,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -850,13 +890,13 @@
         <v>25</v>
       </c>
       <c r="C13">
-        <v>0.57</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="D13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -870,7 +910,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -878,13 +918,13 @@
         <v>27</v>
       </c>
       <c r="C15">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -898,7 +938,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -912,7 +952,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -926,7 +966,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -940,7 +980,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -954,7 +994,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -968,7 +1008,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -982,7 +1022,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -996,7 +1036,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1010,7 +1050,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1024,7 +1064,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1038,7 +1078,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1052,7 +1092,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1060,13 +1100,13 @@
         <v>40</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1074,13 +1114,13 @@
         <v>41</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D29" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1088,13 +1128,13 @@
         <v>42</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="D30" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1108,7 +1148,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1122,7 +1162,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1136,7 +1176,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1150,7 +1190,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1164,7 +1204,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1178,7 +1218,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1192,7 +1232,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -1206,7 +1246,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -1220,7 +1260,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1234,194 +1274,194 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="C41">
-        <v>30</v>
+        <v>0.52</v>
       </c>
       <c r="D41" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D42" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C44">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D44" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>10</v>
       </c>
       <c r="B45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45">
+        <v>150</v>
+      </c>
+      <c r="D45" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
         <v>57</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <v>80</v>
       </c>
-      <c r="D45" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
+      <c r="D46" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>11</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>58</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>69</v>
       </c>
-      <c r="D46" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
-        <v>12</v>
-      </c>
-      <c r="B47" t="s">
-        <v>59</v>
-      </c>
-      <c r="C47">
-        <v>1.6</v>
-      </c>
       <c r="D47" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C48">
-        <v>50</v>
+        <v>1.6</v>
       </c>
       <c r="D48" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C49">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D49" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C50">
-        <v>0.015</v>
+        <v>100</v>
       </c>
       <c r="D50" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C51">
-        <v>0.062</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D51" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C52">
-        <v>500</v>
+        <v>6.2E-2</v>
       </c>
       <c r="D52" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>65</v>
-      </c>
-      <c r="C53" t="s">
-        <v>70</v>
+        <v>64</v>
+      </c>
+      <c r="C53">
+        <v>500</v>
       </c>
       <c r="D53" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" t="s">
         <v>70</v>
@@ -1430,31 +1470,45 @@
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>12</v>
       </c>
       <c r="B55" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" t="s">
         <v>67</v>
       </c>
-      <c r="C55">
+      <c r="C56">
         <v>24</v>
       </c>
-      <c r="D55" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
+      <c r="D56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>13</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>68</v>
       </c>
-      <c r="C56">
+      <c r="C57">
         <v>25</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New updates to scenario methods and supporting data inputs
</commit_message>
<xml_diff>
--- a/data/parameters_config/project_parameters.xlsx
+++ b/data/parameters_config/project_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhartwell/PycharmProjects/VITRIFY/data/parameters_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A099CE67-489A-4C4D-B5F2-B67F4C7D7B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D359814-5DE9-3F42-9088-123D57C3BEBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="105">
   <si>
     <t>Category</t>
   </si>
@@ -272,15 +272,6 @@
     <t>Embodied Carbon: Generic Sealant (kgCO2e/kg)</t>
   </si>
   <si>
-    <t>Embodied Carbon: Aluminium Spacer (kgCO2e/kg)</t>
-  </si>
-  <si>
-    <t>Embodied Carbon: Steel Spacer (kgCO2e/kg)</t>
-  </si>
-  <si>
-    <t>Embodied Carbon: Swiss Spacer (kgCO2e/kg)</t>
-  </si>
-  <si>
     <t>Emissions for disassembly process per m2</t>
   </si>
   <si>
@@ -308,12 +299,6 @@
     <t>Yield loss during disassembly for repurpose (0.0-1.0)</t>
   </si>
   <si>
-    <t>Yield loss during disassembly for reuse (0.0-1.0)</t>
-  </si>
-  <si>
-    <t>Yield loss during repair process (0.0-1.0)</t>
-  </si>
-  <si>
     <t>Backhaul adjustment factor (&gt;1.0)</t>
   </si>
   <si>
@@ -336,6 +321,33 @@
   </si>
   <si>
     <t>Embodied Carbon: Reprocessing Flat Glass (kgCO2e/kg)</t>
+  </si>
+  <si>
+    <t>Embodied Carbon: Aluminium Spacer (kgCO2e/linearmetre)</t>
+  </si>
+  <si>
+    <t>Yield loss during disassembly for component reuse (0.0-1.0)</t>
+  </si>
+  <si>
+    <t>YIELD_SYSTEM_REUSE</t>
+  </si>
+  <si>
+    <t>Yield loss associated with system reuse (0.0-1.0)</t>
+  </si>
+  <si>
+    <t>Yield loss during repair process for system repair (0.0-1.0)</t>
+  </si>
+  <si>
+    <t>Parameter for logic calculation - used for reconditioning components</t>
+  </si>
+  <si>
+    <t>YIELD_DISASSEMBLY_REMANUFACTURE</t>
+  </si>
+  <si>
+    <t>Yield loss during disassembly for remanufacture (0.0-1.0)</t>
+  </si>
+  <si>
+    <t>Parameter for logic calculation (kgCO2/cavity Argon fill)</t>
   </si>
 </sst>
 </file>
@@ -394,11 +406,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,14 +716,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -820,7 +834,7 @@
         <v>20</v>
       </c>
       <c r="C8">
-        <v>0.05</v>
+        <v>6.4799999999999996E-2</v>
       </c>
       <c r="D8" t="s">
         <v>74</v>
@@ -876,7 +890,7 @@
         <v>24</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>3.51</v>
       </c>
       <c r="D12" t="s">
         <v>78</v>
@@ -893,7 +907,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -907,7 +921,7 @@
         <v>0.17</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -921,7 +935,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1005,7 +1019,7 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1019,7 +1033,7 @@
         <v>0.15</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1047,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1058,10 +1072,10 @@
         <v>37</v>
       </c>
       <c r="C25">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="D25" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1075,7 +1089,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1085,11 +1099,12 @@
       <c r="B27" t="s">
         <v>39</v>
       </c>
-      <c r="C27">
-        <v>1</v>
+      <c r="C27" s="2">
+        <f>0.596*0.03</f>
+        <v>1.788E-2</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1145,7 +1160,7 @@
         <v>0.01</v>
       </c>
       <c r="D31" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1159,7 +1174,7 @@
         <v>0.02</v>
       </c>
       <c r="D32" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1173,7 +1188,7 @@
         <v>0.95</v>
       </c>
       <c r="D33" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1187,7 +1202,7 @@
         <v>0.9</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1195,13 +1210,13 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="C35">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D35" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1209,13 +1224,13 @@
         <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C36">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1223,41 +1238,41 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C37">
         <v>0.2</v>
       </c>
       <c r="D37" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="C38">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="D38" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C39">
         <v>0.1</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1265,10 +1280,10 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C40">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="D40" t="s">
         <v>71</v>
@@ -1279,24 +1294,24 @@
         <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="C41">
-        <v>0.52</v>
+        <v>0.4</v>
       </c>
       <c r="D41" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C42">
-        <v>30</v>
+        <v>0.4</v>
       </c>
       <c r="D42" t="s">
         <v>71</v>
@@ -1304,16 +1319,16 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="D43" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1321,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C44">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D44" t="s">
         <v>71</v>
@@ -1335,10 +1350,10 @@
         <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C45">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>71</v>
@@ -1349,10 +1364,10 @@
         <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C46">
-        <v>80</v>
+        <v>1000</v>
       </c>
       <c r="D46" t="s">
         <v>71</v>
@@ -1360,13 +1375,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47" t="s">
-        <v>69</v>
+        <v>56</v>
+      </c>
+      <c r="C47">
+        <v>150</v>
       </c>
       <c r="D47" t="s">
         <v>71</v>
@@ -1374,30 +1389,30 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C48">
-        <v>1.6</v>
+        <v>80</v>
       </c>
       <c r="D48" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>60</v>
-      </c>
-      <c r="C49">
-        <v>50</v>
+        <v>58</v>
+      </c>
+      <c r="C49" t="s">
+        <v>69</v>
       </c>
       <c r="D49" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1405,13 +1420,13 @@
         <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C50">
-        <v>100</v>
+        <v>1.6</v>
       </c>
       <c r="D50" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1419,13 +1434,13 @@
         <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C51">
-        <v>1.4999999999999999E-2</v>
+        <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1433,13 +1448,13 @@
         <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C52">
-        <v>6.2E-2</v>
+        <v>50</v>
       </c>
       <c r="D52" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1447,13 +1462,13 @@
         <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C53">
-        <v>500</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D53" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1461,13 +1476,13 @@
         <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>65</v>
-      </c>
-      <c r="C54" t="s">
-        <v>70</v>
+        <v>63</v>
+      </c>
+      <c r="C54">
+        <v>6.2E-2</v>
       </c>
       <c r="D54" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1475,10 +1490,10 @@
         <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
-      </c>
-      <c r="C55" t="s">
-        <v>70</v>
+        <v>64</v>
+      </c>
+      <c r="C55">
+        <v>500</v>
       </c>
       <c r="D55" t="s">
         <v>71</v>
@@ -1489,10 +1504,10 @@
         <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>67</v>
-      </c>
-      <c r="C56">
-        <v>24</v>
+        <v>65</v>
+      </c>
+      <c r="C56" t="s">
+        <v>70</v>
       </c>
       <c r="D56" t="s">
         <v>71</v>
@@ -1500,16 +1515,44 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58">
+        <v>24</v>
+      </c>
+      <c r="D58" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>13</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B59" t="s">
         <v>68</v>
       </c>
-      <c r="C57">
+      <c r="C59">
         <v>25</v>
       </c>
-      <c r="D57" t="s">
-        <v>98</v>
+      <c r="D59" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>